<commit_message>
fix sample cookies for chrome accessed via database
</commit_message>
<xml_diff>
--- a/cookies/cookies_data_chrome_database.xlsx
+++ b/cookies/cookies_data_chrome_database.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>creation_utc</t>
   </si>
@@ -74,6 +74,30 @@
   </si>
   <si>
     <t>has_cross_site_ancestor</t>
+  </si>
+  <si>
+    <t>www.pineconedata.com</t>
+  </si>
+  <si>
+    <t>sampleCookie1</t>
+  </si>
+  <si>
+    <t>sampleCookie2</t>
+  </si>
+  <si>
+    <t>sampleCookie3</t>
+  </si>
+  <si>
+    <t>b"v10\xdcj\r\xe3m7\x17\x03b\xb7\xc7\xbe\x03\xf5t#\x03Z\n\xa8\xcd\xf6\xade\xf1\x05\x95\x0c\x88\xfc:\xd4\x91\x87|\xd7\xac\xdeG\x1c=\xbe\x97\x113\xa7}a\x12\x13\r\xde\xbbY\x82\x97n\xe9\xbd\xae\x8eW'\x02"</t>
+  </si>
+  <si>
+    <t>b'v10\xdcj\r\xe3m7\x17\x03b\xb7\xc7\xbe\x03\xf5t#\x03Z\n\xa8\xcd\xf6\xade\xf1\x05\x95\x0c\x88\xfc:\xd4$\x9a\xccsg-\xc4\xc6\\2y\xdf\x83D\x1afz=\x99\xbb2\xc4MVIgw\xe6\xc7\xb3\x1fS|\x9d\xed\xc2\xfdw\x8c/]@|\x92_j3S'</t>
+  </si>
+  <si>
+    <t>b'v10\xdcj\r\xe3m7\x17\x03b\xb7\xc7\xbe\x03\xf5t#\x03Z\n\xa8\xcd\xf6\xade\xf1\x05\x95\x0c\x88\xfc:\xd4\xbe\xfe\x98\x89\xc4x\x96\x96t\x12\x88^\x97F#E\xed\xa77\xf2\n\xd6\\2\x01\x9d\x98\x13\xa3\xd0t\x14'</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -431,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -499,6 +523,174 @@
         <v>19</v>
       </c>
     </row>
+    <row r="2" spans="1:20">
+      <c r="A2">
+        <v>1.337997154359603E+16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>1.3380146637E+16</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>443</v>
+      </c>
+      <c r="R2">
+        <v>1.337997154359596E+16</v>
+      </c>
+      <c r="S2">
+        <v>3</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3">
+        <v>1.337997154359825E+16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3">
+        <v>1.33801467E+16</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>443</v>
+      </c>
+      <c r="R3">
+        <v>1.337997154359821E+16</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4">
+        <v>1.33799715436005E+16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>443</v>
+      </c>
+      <c r="R4">
+        <v>1.337997154360046E+16</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update formatting of sample cookies
</commit_message>
<xml_diff>
--- a/cookies/cookies_data_chrome_database.xlsx
+++ b/cookies/cookies_data_chrome_database.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>creation_utc</t>
   </si>
@@ -98,12 +98,27 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Lax</t>
+  </si>
+  <si>
+    <t>Strict</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -156,11 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,8 +540,8 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2">
-        <v>1.337997154359603E+16</v>
+      <c r="A2" s="2">
+        <v>45656.01955134795</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -539,29 +555,26 @@
       <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="H2">
-        <v>1.3380146637E+16</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
+      <c r="H2" s="2">
+        <v>45657.80829861111</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
       </c>
       <c r="P2">
         <v>2</v>
@@ -569,19 +582,19 @@
       <c r="Q2">
         <v>443</v>
       </c>
-      <c r="R2">
-        <v>1.337997154359596E+16</v>
+      <c r="R2" s="2">
+        <v>45656.01955134718</v>
       </c>
       <c r="S2">
         <v>3</v>
       </c>
-      <c r="T2">
+      <c r="T2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3">
-        <v>1.337997154359825E+16</v>
+      <c r="A3" s="2">
+        <v>45656.01955137827</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -595,29 +608,26 @@
       <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="H3">
-        <v>1.33801467E+16</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
+      <c r="H3" s="2">
+        <v>45657.80902777778</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
       </c>
       <c r="P3">
         <v>2</v>
@@ -625,19 +635,19 @@
       <c r="Q3">
         <v>443</v>
       </c>
-      <c r="R3">
-        <v>1.337997154359821E+16</v>
+      <c r="R3" s="2">
+        <v>45656.01955137773</v>
       </c>
       <c r="S3">
         <v>3</v>
       </c>
-      <c r="T3">
+      <c r="T3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4">
-        <v>1.33799715436005E+16</v>
+      <c r="A4" s="2">
+        <v>45656.01955140649</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -651,29 +661,23 @@
       <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="H4">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
         <v>0</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
+      <c r="M4" t="b">
         <v>0</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>31</v>
       </c>
       <c r="P4">
         <v>2</v>
@@ -681,13 +685,13 @@
       <c r="Q4">
         <v>443</v>
       </c>
-      <c r="R4">
-        <v>1.337997154360046E+16</v>
+      <c r="R4" s="2">
+        <v>45656.01955140598</v>
       </c>
       <c r="S4">
         <v>3</v>
       </c>
-      <c r="T4">
+      <c r="T4" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update example files with latest formatting changes
</commit_message>
<xml_diff>
--- a/cookies/cookies_data_chrome_database.xlsx
+++ b/cookies/cookies_data_chrome_database.xlsx
@@ -14,66 +14,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
-  <si>
-    <t>creation_utc</t>
-  </si>
-  <si>
-    <t>host_key</t>
-  </si>
-  <si>
-    <t>top_frame_site_key</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+  <si>
+    <t>creationTime</t>
+  </si>
+  <si>
+    <t>host</t>
   </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>encrypted_value</t>
-  </si>
-  <si>
     <t>path</t>
   </si>
   <si>
-    <t>expires_utc</t>
-  </si>
-  <si>
-    <t>is_secure</t>
-  </si>
-  <si>
-    <t>is_httponly</t>
-  </si>
-  <si>
-    <t>last_access_utc</t>
-  </si>
-  <si>
-    <t>has_expires</t>
-  </si>
-  <si>
-    <t>is_persistent</t>
+    <t>expiry</t>
+  </si>
+  <si>
+    <t>isSecure</t>
+  </si>
+  <si>
+    <t>isHttpOnly</t>
+  </si>
+  <si>
+    <t>lastAccessedTime</t>
+  </si>
+  <si>
+    <t>hasExpires</t>
+  </si>
+  <si>
+    <t>isPersistent</t>
   </si>
   <si>
     <t>priority</t>
   </si>
   <si>
-    <t>samesite</t>
-  </si>
-  <si>
-    <t>source_scheme</t>
-  </si>
-  <si>
-    <t>source_port</t>
-  </si>
-  <si>
-    <t>last_update_utc</t>
-  </si>
-  <si>
-    <t>source_type</t>
-  </si>
-  <si>
-    <t>has_cross_site_ancestor</t>
+    <t>sourceScheme</t>
+  </si>
+  <si>
+    <t>sourcePort</t>
+  </si>
+  <si>
+    <t>lastUpdatedTime</t>
+  </si>
+  <si>
+    <t>sourceType</t>
+  </si>
+  <si>
+    <t>hasCrossSiteAncestor</t>
+  </si>
+  <si>
+    <t>sameSite</t>
+  </si>
+  <si>
+    <t>decryptedValue</t>
   </si>
   <si>
     <t>www.pineconedata.com</t>
@@ -88,18 +82,12 @@
     <t>sampleCookie3</t>
   </si>
   <si>
-    <t>b"v10\xdcj\r\xe3m7\x17\x03b\xb7\xc7\xbe\x03\xf5t#\x03Z\n\xa8\xcd\xf6\xade\xf1\x05\x95\x0c\x88\xfc:\xd4\x91\x87|\xd7\xac\xdeG\x1c=\xbe\x97\x113\xa7}a\x12\x13\r\xde\xbbY\x82\x97n\xe9\xbd\xae\x8eW'\x02"</t>
-  </si>
-  <si>
-    <t>b'v10\xdcj\r\xe3m7\x17\x03b\xb7\xc7\xbe\x03\xf5t#\x03Z\n\xa8\xcd\xf6\xade\xf1\x05\x95\x0c\x88\xfc:\xd4$\x9a\xccsg-\xc4\xc6\\2y\xdf\x83D\x1afz=\x99\xbb2\xc4MVIgw\xe6\xc7\xb3\x1fS|\x9d\xed\xc2\xfdw\x8c/]@|\x92_j3S'</t>
-  </si>
-  <si>
-    <t>b'v10\xdcj\r\xe3m7\x17\x03b\xb7\xc7\xbe\x03\xf5t#\x03Z\n\xa8\xcd\xf6\xade\xf1\x05\x95\x0c\x88\xfc:\xd4\xbe\xfe\x98\x89\xc4x\x96\x96t\x12\x88^\x97F#E\xed\xa77\xf2\n\xd6\\2\x01\x9d\x98\x13\xa3\xd0t\x14'</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
+    <t>session</t>
+  </si>
+  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -110,6 +98,15 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>this is a secure sample cookie</t>
+  </si>
+  <si>
+    <t>this is a HTTP Only sample cookie</t>
+  </si>
+  <si>
+    <t>this is another sample cookie</t>
   </si>
 </sst>
 </file>
@@ -471,13 +468,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,167 +529,164 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2">
+        <v>45663.9679170036</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45671.17625</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>443</v>
+      </c>
+      <c r="N2" s="2">
+        <v>45663.96791700294</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="2">
-        <v>45656.01955134795</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2">
-        <v>45657.80829861111</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2">
-        <v>2</v>
-      </c>
-      <c r="Q2">
-        <v>443</v>
-      </c>
-      <c r="R2" s="2">
-        <v>45656.01955134718</v>
-      </c>
-      <c r="S2">
-        <v>3</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:18">
       <c r="A3" s="2">
-        <v>45656.01955137827</v>
+        <v>45663.96791702352</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E3" s="2">
+        <v>45694.17625</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>443</v>
+      </c>
+      <c r="N3" s="2">
+        <v>45663.96791702318</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="2">
+        <v>45663.96791704138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>443</v>
+      </c>
+      <c r="N4" s="2">
+        <v>45663.96791704107</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="2">
-        <v>45657.80902777778</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="R4" t="s">
         <v>30</v>
-      </c>
-      <c r="P3">
-        <v>2</v>
-      </c>
-      <c r="Q3">
-        <v>443</v>
-      </c>
-      <c r="R3" s="2">
-        <v>45656.01955137773</v>
-      </c>
-      <c r="S3">
-        <v>3</v>
-      </c>
-      <c r="T3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="2">
-        <v>45656.01955140649</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>443</v>
-      </c>
-      <c r="R4" s="2">
-        <v>45656.01955140598</v>
-      </c>
-      <c r="S4">
-        <v>3</v>
-      </c>
-      <c r="T4" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update example files to reflect source scheme and source type formatting changes
</commit_message>
<xml_diff>
--- a/cookies/cookies_data_chrome_database.xlsx
+++ b/cookies/cookies_data_chrome_database.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>creationTime</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>Secure</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
   <si>
     <t>Lax</t>
@@ -532,7 +538,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="2">
-        <v>45663.9679170036</v>
+        <v>45664.23578169493</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -544,7 +550,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2">
-        <v>45671.17625</v>
+        <v>45671.4441087963</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -561,31 +567,31 @@
       <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="L2">
-        <v>2</v>
+      <c r="L2" t="s">
+        <v>25</v>
       </c>
       <c r="M2">
         <v>443</v>
       </c>
       <c r="N2" s="2">
-        <v>45663.96791700294</v>
-      </c>
-      <c r="O2">
-        <v>3</v>
+        <v>45664.23578169434</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
       </c>
       <c r="P2" t="b">
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="2">
-        <v>45663.96791702352</v>
+        <v>45664.23578172098</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -597,7 +603,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="2">
-        <v>45694.17625</v>
+        <v>45694.4441087963</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -614,31 +620,31 @@
       <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="L3">
-        <v>2</v>
+      <c r="L3" t="s">
+        <v>25</v>
       </c>
       <c r="M3">
         <v>443</v>
       </c>
       <c r="N3" s="2">
-        <v>45663.96791702318</v>
-      </c>
-      <c r="O3">
-        <v>3</v>
+        <v>45664.23578172042</v>
+      </c>
+      <c r="O3" t="s">
+        <v>26</v>
       </c>
       <c r="P3" t="b">
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="2">
-        <v>45663.96791704138</v>
+        <v>45664.23578176276</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -667,26 +673,26 @@
       <c r="K4" t="s">
         <v>24</v>
       </c>
-      <c r="L4">
-        <v>2</v>
+      <c r="L4" t="s">
+        <v>25</v>
       </c>
       <c r="M4">
         <v>443</v>
       </c>
       <c r="N4" s="2">
-        <v>45663.96791704107</v>
-      </c>
-      <c r="O4">
-        <v>3</v>
+        <v>45664.23578176225</v>
+      </c>
+      <c r="O4" t="s">
+        <v>26</v>
       </c>
       <c r="P4" t="b">
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="R4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>